<commit_message>
removed machine_name_references and started using ui_lookup
</commit_message>
<xml_diff>
--- a/data-raw/test-map_metadata_excel.xlsx
+++ b/data-raw/test-map_metadata_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb525812\cmder\Git Repos\ddhconnect\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{173A5A19-1A44-49C9-8F57-9C8C4DE1760E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D80FB867-49C5-4F48-90F3-02FBBA90E840}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,13 +40,13 @@
     <t>Test Body</t>
   </si>
   <si>
-    <t>TTL Name/ UPI</t>
-  </si>
-  <si>
     <t>WARNING</t>
   </si>
   <si>
     <t>MISS</t>
+  </si>
+  <si>
+    <t>TTL Name or UPI</t>
   </si>
 </sst>
 </file>
@@ -890,12 +890,12 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -925,7 +925,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>46404</v>
@@ -933,10 +933,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>